<commit_message>
Vector review and course timeline updates
</commit_message>
<xml_diff>
--- a/0_CERTIFICATES/Courses_Sheet.xlsx
+++ b/0_CERTIFICATES/Courses_Sheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SYED\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\0_CERTIFICATES\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D693C2A-43C6-4CB9-9961-9CB588D05704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7635"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COURSERA_PLUS" sheetId="2" r:id="rId1"/>
@@ -17,17 +18,27 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">COURSERA_PLUS!$B$4:$H$9</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
   <si>
     <t>COURSERA Plus Courses</t>
   </si>
@@ -38,9 +49,6 @@
     <t>Updated:</t>
   </si>
   <si>
-    <t>2022 - 06 - 27</t>
-  </si>
-  <si>
     <t>Sr. #</t>
   </si>
   <si>
@@ -138,12 +146,15 @@
   </si>
   <si>
     <t>Building Arduino robots and devices</t>
+  </si>
+  <si>
+    <t>2022 - 06 - 28</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -178,56 +189,56 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF002060"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF7030A0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF008000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <i/>
       <sz val="8"/>
-      <color rgb="FF00B050"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF00B050"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF002060"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="8" tint="-0.499984740745262"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF7030A0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF008000"/>
+      <color rgb="FFC00000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -275,11 +286,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -288,16 +298,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -305,6 +315,9 @@
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -586,14 +599,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF99FF33"/>
   </sheetPr>
   <dimension ref="B2:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -614,393 +627,393 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="G3" s="5" t="s">
+      <c r="C3" s="3"/>
+      <c r="G3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>1</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="12">
+        <v>2022</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="9">
+        <v>2</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G6" s="14">
+      <c r="D7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="12">
+        <v>2022</v>
+      </c>
+      <c r="G7" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="10">
-        <v>2</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="12" t="s">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="9">
+        <v>3</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G7" s="14">
+      <c r="D8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="12">
+        <v>2022</v>
+      </c>
+      <c r="G8" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="10">
-        <v>3</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G8" s="14">
-        <v>1</v>
-      </c>
-    </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <f t="shared" ref="B9:B22" ca="1" si="0">IFERROR(OFFSET(B9,-1,0,1,1)+1,"")</f>
         <v>4</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G9" s="14">
+      <c r="F9" s="12">
+        <v>2022</v>
+      </c>
+      <c r="G9" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="10">
-        <f t="shared" ca="1" si="0"/>
+      <c r="B10" s="9">
+        <f ca="1">IFERROR(OFFSET(B10,-1,0,1,1)+1,"")</f>
         <v>5</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>22</v>
+      <c r="C10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="12">
+        <v>2022</v>
+      </c>
+      <c r="G10" s="15">
+        <v>0.66</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="10">
-        <f t="shared" ca="1" si="0"/>
+      <c r="B11" s="9">
+        <f ca="1">IFERROR(OFFSET(B11,-1,0,1,1)+1,"")</f>
         <v>6</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G11" s="16">
-        <v>0.08</v>
+      <c r="C11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="12">
+        <v>2022</v>
+      </c>
+      <c r="G11" s="15">
+        <v>0.13</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="10">
-        <f t="shared" ca="1" si="0"/>
+      <c r="B12" s="9">
+        <f ca="1">IFERROR(OFFSET(B12,-1,0,1,1)+1,"")</f>
         <v>7</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G12" s="16">
-        <v>0.66</v>
+      <c r="D12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="12">
+        <v>2022</v>
+      </c>
+      <c r="G12" s="15">
+        <v>0.34</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="12">
+        <v>2022</v>
+      </c>
+      <c r="G13" s="14">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="9">
+        <f ca="1">IFERROR(OFFSET(B14,-1,0,1,1)+1,"")</f>
+        <v>9</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="12">
+        <v>2022</v>
+      </c>
+      <c r="G14" s="15">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="9">
+        <f ca="1">IFERROR(OFFSET(B15,-1,0,1,1)+1,"")</f>
+        <v>10</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="12">
+        <v>2022</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="9">
+        <f ca="1">IFERROR(OFFSET(B16,-1,0,1,1)+1,"")</f>
+        <v>11</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="12">
+        <v>2022</v>
+      </c>
+      <c r="G16" s="15">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="9">
+        <f ca="1">IFERROR(OFFSET(B17,-1,0,1,1)+1,"")</f>
+        <v>12</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="12">
+        <v>2022</v>
+      </c>
+      <c r="G17" s="15">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="9">
+        <f ca="1">IFERROR(OFFSET(B18,-1,0,1,1)+1,"")</f>
+        <v>13</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="12">
+        <v>2022</v>
+      </c>
+      <c r="G18" s="15">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="12">
+        <v>2022</v>
+      </c>
+      <c r="G19" s="15">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="9">
+        <f ca="1">IFERROR(OFFSET(B20,-1,0,1,1)+1,"")</f>
         <v>15</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G13" s="16">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G14" s="16">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G15" s="16">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C17" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G18" s="16">
+      <c r="D20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="12">
+        <v>2022</v>
+      </c>
+      <c r="G20" s="15">
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G20" s="16">
-        <v>0.35</v>
-      </c>
-    </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="10">
+      <c r="B21" s="9">
         <f t="shared" ca="1" si="0"/>
         <v>16</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>22</v>
+      <c r="C21" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="12">
+        <v>2022</v>
+      </c>
+      <c r="G21" s="15">
+        <v>0.17</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="10">
+      <c r="B22" s="9">
         <f t="shared" ca="1" si="0"/>
         <v>17</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>22</v>
+      <c r="C22" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="12">
+        <v>2022</v>
+      </c>
+      <c r="G22" s="15">
+        <v>0.24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>